<commit_message>
Arreglado Cogstate (celdas en blanco) y pacientes mayores.
</commit_message>
<xml_diff>
--- a/TFG/res/pacientData/13006/Resultats_REM-G13006.xlsx
+++ b/TFG/res/pacientData/13006/Resultats_REM-G13006.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1004" uniqueCount="606">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1004" uniqueCount="626">
   <si>
     <t>ID</t>
   </si>
@@ -1682,7 +1682,7 @@
     <t>Català i castellà</t>
   </si>
   <si>
-    <t>25/02/1941</t>
+    <t>25/02/1931</t>
   </si>
   <si>
     <t>Estudis primaris no finalitzats</t>
@@ -1736,9 +1736,87 @@
     <t>10</t>
   </si>
   <si>
+    <t>23075</t>
+  </si>
+  <si>
+    <t>0.61548</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>31857</t>
+  </si>
+  <si>
+    <t>0.78540</t>
+  </si>
+  <si>
+    <t>37185</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>38</t>
+  </si>
+  <si>
+    <t>0.00000</t>
+  </si>
+  <si>
+    <t>50</t>
+  </si>
+  <si>
+    <t>36</t>
+  </si>
+  <si>
+    <t>52</t>
+  </si>
+  <si>
+    <t>318104</t>
+  </si>
+  <si>
+    <t>0.16336</t>
+  </si>
+  <si>
+    <t>0.69398</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>322266</t>
+  </si>
+  <si>
+    <t>0.10278</t>
+  </si>
+  <si>
+    <t>0.44051</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>27</t>
+  </si>
+  <si>
+    <t>390424</t>
+  </si>
+  <si>
+    <t>0.18649</t>
+  </si>
+  <si>
+    <t>0.71065</t>
+  </si>
+  <si>
     <t>7</t>
   </si>
   <si>
+    <t>0.86912</t>
+  </si>
+  <si>
+    <t>67830</t>
+  </si>
+  <si>
     <t>175</t>
   </si>
   <si>
@@ -1763,15 +1841,9 @@
     <t>00:45.41</t>
   </si>
   <si>
-    <t>20</t>
-  </si>
-  <si>
     <t>00:45.38</t>
   </si>
   <si>
-    <t>1</t>
-  </si>
-  <si>
     <t>01:34.87</t>
   </si>
   <si>
@@ -1781,9 +1853,6 @@
     <t>02:01.26</t>
   </si>
   <si>
-    <t>8</t>
-  </si>
-  <si>
     <t>16</t>
   </si>
   <si>
@@ -1802,15 +1871,9 @@
     <t>41</t>
   </si>
   <si>
-    <t>38</t>
-  </si>
-  <si>
     <t>68</t>
   </si>
   <si>
-    <t>52</t>
-  </si>
-  <si>
     <t>40</t>
   </si>
   <si>
@@ -1827,9 +1890,6 @@
   </si>
   <si>
     <t>25</t>
-  </si>
-  <si>
-    <t>12</t>
   </si>
 </sst>
 </file>
@@ -4497,55 +4557,55 @@
         <v>573</v>
       </c>
       <c r="HR2" t="s">
-        <v>137</v>
+        <v>574</v>
       </c>
       <c r="HS2" t="s">
-        <v>137</v>
+        <v>575</v>
       </c>
       <c r="HT2" t="s">
-        <v>137</v>
+        <v>568</v>
       </c>
       <c r="HU2" t="s">
-        <v>137</v>
+        <v>570</v>
       </c>
       <c r="HV2" t="s">
-        <v>137</v>
+        <v>576</v>
       </c>
       <c r="HW2" t="s">
-        <v>137</v>
+        <v>577</v>
       </c>
       <c r="HX2" t="s">
-        <v>137</v>
+        <v>578</v>
       </c>
       <c r="HY2" t="s">
-        <v>137</v>
+        <v>558</v>
       </c>
       <c r="HZ2" t="s">
-        <v>137</v>
+        <v>570</v>
       </c>
       <c r="IA2" t="s">
-        <v>137</v>
+        <v>576</v>
       </c>
       <c r="IB2" t="s">
-        <v>137</v>
+        <v>579</v>
       </c>
       <c r="IC2" t="s">
-        <v>137</v>
+        <v>578</v>
       </c>
       <c r="ID2" t="s">
-        <v>137</v>
+        <v>558</v>
       </c>
       <c r="IE2" t="s">
-        <v>137</v>
+        <v>580</v>
       </c>
       <c r="IF2" t="s">
-        <v>137</v>
+        <v>576</v>
       </c>
       <c r="IG2" t="s">
-        <v>137</v>
+        <v>570</v>
       </c>
       <c r="IH2" t="s">
-        <v>137</v>
+        <v>581</v>
       </c>
       <c r="II2" t="s">
         <v>137</v>
@@ -4554,13 +4614,13 @@
         <v>137</v>
       </c>
       <c r="IK2" t="s">
-        <v>137</v>
+        <v>582</v>
       </c>
       <c r="IL2" t="s">
-        <v>137</v>
+        <v>570</v>
       </c>
       <c r="IM2" t="s">
-        <v>137</v>
+        <v>583</v>
       </c>
       <c r="IN2" t="s">
         <v>137</v>
@@ -4569,67 +4629,67 @@
         <v>137</v>
       </c>
       <c r="IP2" t="s">
-        <v>137</v>
+        <v>582</v>
       </c>
       <c r="IQ2" t="s">
-        <v>137</v>
+        <v>584</v>
       </c>
       <c r="IR2" t="s">
-        <v>137</v>
+        <v>585</v>
       </c>
       <c r="IS2" t="s">
-        <v>137</v>
+        <v>586</v>
       </c>
       <c r="IT2" t="s">
-        <v>137</v>
+        <v>587</v>
       </c>
       <c r="IU2" t="s">
-        <v>137</v>
+        <v>588</v>
       </c>
       <c r="IV2" t="s">
-        <v>137</v>
+        <v>589</v>
       </c>
       <c r="IW2" t="s">
-        <v>137</v>
+        <v>584</v>
       </c>
       <c r="IX2" t="s">
-        <v>137</v>
+        <v>590</v>
       </c>
       <c r="IY2" t="s">
-        <v>137</v>
+        <v>591</v>
       </c>
       <c r="IZ2" t="s">
-        <v>137</v>
+        <v>592</v>
       </c>
       <c r="JA2" t="s">
-        <v>137</v>
+        <v>593</v>
       </c>
       <c r="JB2" t="s">
-        <v>137</v>
+        <v>594</v>
       </c>
       <c r="JC2" t="s">
-        <v>137</v>
+        <v>595</v>
       </c>
       <c r="JD2" t="s">
-        <v>137</v>
+        <v>596</v>
       </c>
       <c r="JE2" t="s">
-        <v>137</v>
+        <v>597</v>
       </c>
       <c r="JF2" t="s">
-        <v>137</v>
+        <v>598</v>
       </c>
       <c r="JG2" t="s">
-        <v>137</v>
+        <v>580</v>
       </c>
       <c r="JH2" t="s">
-        <v>137</v>
+        <v>599</v>
       </c>
       <c r="JI2" t="s">
-        <v>137</v>
+        <v>600</v>
       </c>
       <c r="JJ2" t="s">
-        <v>574</v>
+        <v>598</v>
       </c>
       <c r="JK2" t="s">
         <v>573</v>
@@ -4650,37 +4710,37 @@
         <v>570</v>
       </c>
       <c r="JQ2" t="s">
-        <v>575</v>
+        <v>601</v>
       </c>
       <c r="JR2" t="s">
-        <v>576</v>
+        <v>602</v>
       </c>
       <c r="JS2" t="s">
-        <v>577</v>
+        <v>603</v>
       </c>
       <c r="JT2" t="s">
-        <v>578</v>
+        <v>604</v>
       </c>
       <c r="JU2" t="s">
         <v>570</v>
       </c>
       <c r="JV2" t="s">
-        <v>579</v>
+        <v>605</v>
       </c>
       <c r="JW2" t="s">
         <v>570</v>
       </c>
       <c r="JX2" t="s">
-        <v>579</v>
+        <v>605</v>
       </c>
       <c r="JY2" t="s">
         <v>570</v>
       </c>
       <c r="JZ2" t="s">
-        <v>579</v>
+        <v>605</v>
       </c>
       <c r="KA2" t="s">
-        <v>580</v>
+        <v>606</v>
       </c>
       <c r="KB2" t="s">
         <v>137</v>
@@ -4695,31 +4755,31 @@
         <v>570</v>
       </c>
       <c r="KF2" t="s">
-        <v>579</v>
+        <v>605</v>
       </c>
       <c r="KG2" t="s">
         <v>570</v>
       </c>
       <c r="KH2" t="s">
-        <v>579</v>
+        <v>605</v>
       </c>
       <c r="KI2" t="s">
         <v>570</v>
       </c>
       <c r="KJ2" t="s">
-        <v>579</v>
+        <v>605</v>
       </c>
       <c r="KK2" t="s">
-        <v>581</v>
+        <v>607</v>
       </c>
       <c r="KL2" t="s">
-        <v>579</v>
+        <v>605</v>
       </c>
       <c r="KM2" t="s">
-        <v>582</v>
+        <v>608</v>
       </c>
       <c r="KN2" t="s">
-        <v>583</v>
+        <v>593</v>
       </c>
       <c r="KO2" t="s">
         <v>570</v>
@@ -4728,22 +4788,22 @@
         <v>137</v>
       </c>
       <c r="KQ2" t="s">
-        <v>584</v>
+        <v>609</v>
       </c>
       <c r="KR2" t="s">
-        <v>583</v>
+        <v>593</v>
       </c>
       <c r="KS2" t="s">
-        <v>585</v>
+        <v>580</v>
       </c>
       <c r="KT2" t="s">
         <v>137</v>
       </c>
       <c r="KU2" t="s">
-        <v>586</v>
+        <v>610</v>
       </c>
       <c r="KV2" t="s">
-        <v>587</v>
+        <v>611</v>
       </c>
       <c r="KW2" t="s">
         <v>571</v>
@@ -4752,7 +4812,7 @@
         <v>137</v>
       </c>
       <c r="KY2" t="s">
-        <v>588</v>
+        <v>612</v>
       </c>
       <c r="KZ2" t="s">
         <v>569</v>
@@ -4764,7 +4824,7 @@
         <v>137</v>
       </c>
       <c r="LC2" t="s">
-        <v>587</v>
+        <v>611</v>
       </c>
       <c r="LD2" t="s">
         <v>573</v>
@@ -4800,82 +4860,82 @@
         <v>568</v>
       </c>
       <c r="LO2" t="s">
-        <v>590</v>
+        <v>613</v>
       </c>
       <c r="LP2" t="s">
-        <v>591</v>
+        <v>614</v>
       </c>
       <c r="LQ2" t="s">
-        <v>592</v>
+        <v>615</v>
       </c>
       <c r="LR2" t="s">
-        <v>593</v>
+        <v>616</v>
       </c>
       <c r="LS2" t="s">
         <v>572</v>
       </c>
       <c r="LT2" t="s">
-        <v>587</v>
+        <v>611</v>
       </c>
       <c r="LU2" t="s">
-        <v>587</v>
+        <v>611</v>
       </c>
       <c r="LV2" t="s">
-        <v>594</v>
+        <v>617</v>
       </c>
       <c r="LW2" t="s">
-        <v>595</v>
+        <v>618</v>
       </c>
       <c r="LX2" t="s">
         <v>570</v>
       </c>
       <c r="LY2" t="s">
-        <v>596</v>
+        <v>581</v>
       </c>
       <c r="LZ2" t="s">
-        <v>597</v>
+        <v>619</v>
       </c>
       <c r="MA2" t="s">
-        <v>594</v>
+        <v>617</v>
       </c>
       <c r="MB2" t="s">
         <v>572</v>
       </c>
       <c r="MC2" t="s">
-        <v>598</v>
+        <v>585</v>
       </c>
       <c r="MD2" t="s">
-        <v>585</v>
+        <v>580</v>
       </c>
       <c r="ME2" t="s">
-        <v>587</v>
+        <v>611</v>
       </c>
       <c r="MF2" t="s">
-        <v>599</v>
+        <v>620</v>
       </c>
       <c r="MG2" t="s">
         <v>572</v>
       </c>
       <c r="MH2" t="s">
-        <v>600</v>
+        <v>621</v>
       </c>
       <c r="MI2" t="s">
-        <v>600</v>
+        <v>621</v>
       </c>
       <c r="MJ2" t="s">
-        <v>601</v>
+        <v>622</v>
       </c>
       <c r="MK2" t="s">
         <v>137</v>
       </c>
       <c r="ML2" t="s">
-        <v>602</v>
+        <v>623</v>
       </c>
       <c r="MM2" t="s">
         <v>570</v>
       </c>
       <c r="MN2" t="s">
-        <v>583</v>
+        <v>593</v>
       </c>
       <c r="MO2" t="s">
         <v>570</v>
@@ -4884,16 +4944,16 @@
         <v>570</v>
       </c>
       <c r="MQ2" t="s">
-        <v>603</v>
+        <v>624</v>
       </c>
       <c r="MR2" t="s">
         <v>567</v>
       </c>
       <c r="MS2" t="s">
-        <v>604</v>
+        <v>625</v>
       </c>
       <c r="MT2" t="s">
-        <v>605</v>
+        <v>576</v>
       </c>
     </row>
   </sheetData>

</xml_diff>